<commit_message>
Correcciones lógicas y gráficas
</commit_message>
<xml_diff>
--- a/Excel/Clientes.xlsx
+++ b/Excel/Clientes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Nombre</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Historial de pedidos</t>
   </si>
   <si>
-    <t>0,</t>
+    <t>0,7,</t>
   </si>
   <si>
     <t>Alberto Hurtado</t>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>9-38274654</t>
+  </si>
+  <si>
+    <t>6,</t>
+  </si>
+  <si>
+    <t>Javiera Cabrera</t>
+  </si>
+  <si>
+    <t>javieracabrera14@gmail.com</t>
+  </si>
+  <si>
+    <t>9-66666666</t>
   </si>
 </sst>
 </file>
@@ -218,6 +230,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>